<commit_message>
clean up code, run blk7
</commit_message>
<xml_diff>
--- a/scenario_cooling_demands.xlsx
+++ b/scenario_cooling_demands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/414ed677b2b9daa6/Documents/NUS/b3m/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="113" documentId="8_{1165E018-AF16-4AF6-B3D6-4D3A76DDADBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3BEE4F8-1500-42F5-867F-70F7580B0E0D}"/>
+  <xr:revisionPtr revIDLastSave="172" documentId="8_{1165E018-AF16-4AF6-B3D6-4D3A76DDADBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C374F839-3F5B-4FB3-81D2-5DC73F7EBEDE}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D93F7666-A15E-4CFC-9D5B-B910369D1BD2}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{D93F7666-A15E-4CFC-9D5B-B910369D1BD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="14">
   <si>
     <t>North facing façade</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>South facing façade</t>
+  </si>
+  <si>
+    <t>All facades</t>
+  </si>
+  <si>
+    <t>Only include green roof in building level analysis, doesn't make sense as per façade</t>
   </si>
 </sst>
 </file>
@@ -95,7 +101,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,8 +120,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -209,35 +221,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -249,36 +287,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -620,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F4B229-28D8-4EC9-B071-99690BEB9EF1}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -638,43 +661,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="14"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="19"/>
       <c r="J1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="22" t="s">
         <v>9</v>
       </c>
       <c r="J2" t="s">
@@ -682,242 +705,424 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="6">
-        <v>18394.84</v>
-      </c>
-      <c r="C3" s="7">
+      <c r="B3" s="5">
+        <f>18394.84/3</f>
+        <v>6131.6133333333337</v>
+      </c>
+      <c r="C3" s="6">
         <f>(B3-B3)/B3*100</f>
         <v>0</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>0.7</v>
       </c>
-      <c r="E3" s="7">
-        <v>18390.689999999999</v>
-      </c>
-      <c r="F3" s="9">
+      <c r="E3" s="6">
+        <f>18390.69/3</f>
+        <v>6130.23</v>
+      </c>
+      <c r="F3" s="23">
         <v>3</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="23">
         <v>0.15</v>
       </c>
-      <c r="H3" s="10">
-        <v>17633.400000000001</v>
+      <c r="H3" s="24">
+        <f>17633.4/3</f>
+        <v>5877.8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A4" s="17">
+      <c r="A4" s="10">
         <v>0.25</v>
       </c>
-      <c r="B4" s="6">
-        <v>18394.53</v>
-      </c>
-      <c r="C4" s="7">
+      <c r="B4" s="5">
+        <f>18394.53/3</f>
+        <v>6131.5099999999993</v>
+      </c>
+      <c r="C4" s="6">
         <f>(B4-B3)/B3*100</f>
-        <v>-1.6852552128820346E-3</v>
-      </c>
-      <c r="D4" s="6">
+        <v>-1.6852552128919231E-3</v>
+      </c>
+      <c r="D4" s="5">
         <v>0.5</v>
       </c>
-      <c r="E4" s="7">
-        <v>18206.91</v>
-      </c>
-      <c r="F4" s="8">
+      <c r="E4" s="6">
+        <f>18206.91/3</f>
+        <v>6068.97</v>
+      </c>
+      <c r="F4" s="23">
         <v>1.5</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="23">
         <v>1</v>
       </c>
-      <c r="H4" s="7">
-        <v>17729.89</v>
+      <c r="H4" s="24">
+        <f>17729.89/3</f>
+        <v>5909.9633333333331</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A5" s="18">
+      <c r="A5" s="11">
         <v>0.5</v>
       </c>
-      <c r="B5" s="9">
-        <v>18390.689999999999</v>
-      </c>
-      <c r="C5" s="10">
+      <c r="B5" s="7">
+        <f>18390.69/3</f>
+        <v>6130.23</v>
+      </c>
+      <c r="C5" s="8">
         <f>(B5-B3)/B3*100</f>
-        <v>-2.2560674623978545E-2</v>
-      </c>
-      <c r="D5" s="6">
+        <v>-2.2560674623983489E-2</v>
+      </c>
+      <c r="D5" s="5">
         <v>0.4</v>
       </c>
-      <c r="E5" s="7">
-        <v>18106.560000000001</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="7"/>
+      <c r="E5" s="6">
+        <f>18106.56/3</f>
+        <v>6035.52</v>
+      </c>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A6" s="17">
+      <c r="A6" s="10">
         <v>0.75</v>
       </c>
-      <c r="B6" s="6">
-        <v>18385.95</v>
-      </c>
-      <c r="C6" s="7">
+      <c r="B6" s="5">
+        <f>18385.95/3</f>
+        <v>6128.6500000000005</v>
+      </c>
+      <c r="C6" s="6">
         <f>(B6-B3)/B3*100</f>
-        <v>-4.8328770459538754E-2</v>
-      </c>
-      <c r="D6" s="6">
+        <v>-4.8328770459538747E-2</v>
+      </c>
+      <c r="D6" s="5">
         <v>0.3</v>
       </c>
-      <c r="E6" s="7">
-        <v>17998.66</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
+      <c r="E6" s="6">
+        <f>17998.66/3</f>
+        <v>5999.5533333333333</v>
+      </c>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A7" s="19">
+      <c r="A7" s="12">
         <v>1</v>
       </c>
-      <c r="B7" s="20">
-        <v>18381.29</v>
-      </c>
-      <c r="C7" s="21">
+      <c r="B7" s="13">
+        <f>18381.29/3</f>
+        <v>6127.0966666666673</v>
+      </c>
+      <c r="C7" s="14">
         <f>(B7-B3)/B3*100</f>
         <v>-7.3661961724044739E-2</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="15">
         <v>0.2</v>
       </c>
-      <c r="E7" s="23">
-        <v>17881.14</v>
-      </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="21"/>
+      <c r="E7" s="16">
+        <f>17881.14/3</f>
+        <v>5960.38</v>
+      </c>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="26"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="14"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="19"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="16" t="s">
+      <c r="H10" s="22" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="6">
+      <c r="B11" s="5">
+        <f>18394.84/3</f>
+        <v>6131.6133333333337</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="5">
         <v>0.7</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="8">
+      <c r="E11" s="6">
+        <v>6132.1379999999999</v>
+      </c>
+      <c r="F11" s="23">
         <v>3</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="23">
         <v>0.15</v>
       </c>
-      <c r="H11" s="11"/>
+      <c r="H11" s="24">
+        <v>5876.1440000000002</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A12" s="17">
+      <c r="A12" s="10">
         <v>0.25</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="6">
+      <c r="B12" s="5">
+        <v>6131.8180000000002</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="5">
         <v>0.5</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8">
+      <c r="E12" s="6">
+        <v>6070.8680000000004</v>
+      </c>
+      <c r="F12" s="23">
         <v>1.5</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="23">
         <v>1</v>
       </c>
-      <c r="H12" s="7"/>
+      <c r="H12" s="24">
+        <v>5908.5360000000001</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A13" s="24">
+      <c r="A13" s="10">
         <v>0.5</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="6">
+      <c r="B13" s="5">
+        <v>6132.1379999999999</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="5">
         <v>0.4</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="7"/>
+      <c r="E13" s="6">
+        <v>6037.4110000000001</v>
+      </c>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A14" s="17">
+      <c r="A14" s="10">
         <v>0.75</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="6">
+      <c r="B14" s="5">
+        <v>6132.4279999999999</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="5">
         <v>0.3</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="7"/>
+      <c r="E14" s="6">
+        <v>6001.4350000000004</v>
+      </c>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A15" s="19">
+      <c r="A15" s="12">
         <v>1</v>
       </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="25">
+      <c r="B15" s="13">
+        <v>6132.7820000000002</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="13">
         <v>0.2</v>
       </c>
-      <c r="E15" s="26"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="21"/>
+      <c r="E15" s="14">
+        <v>5962.2539999999999</v>
+      </c>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A17" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="19"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A18" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A19" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="5">
+        <f>18394.84/3</f>
+        <v>6131.6133333333337</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="E19" s="20">
+        <v>6130.7489999999998</v>
+      </c>
+      <c r="F19" s="5">
+        <v>3</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="H19" s="6">
+        <v>5876.1409999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A20" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="B20" s="5">
+        <v>6131.7160000000003</v>
+      </c>
+      <c r="C20" s="6"/>
+      <c r="D20" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="6">
+        <v>6069.49</v>
+      </c>
+      <c r="F20" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="G20" s="5">
+        <v>1</v>
+      </c>
+      <c r="H20" s="6">
+        <v>5908.5330000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="B21" s="5">
+        <v>6130.7489999999998</v>
+      </c>
+      <c r="C21" s="6"/>
+      <c r="D21" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="E21" s="6">
+        <v>6036.0379999999996</v>
+      </c>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A22" s="10">
+        <v>0.75</v>
+      </c>
+      <c r="B22" s="5">
+        <v>6129.45</v>
+      </c>
+      <c r="C22" s="6"/>
+      <c r="D22" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="E22" s="6">
+        <v>6000.0720000000001</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A23" s="12">
+        <v>1</v>
+      </c>
+      <c r="B23" s="13">
+        <v>6128.2489999999998</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="E23" s="14">
+        <v>5960.8990000000003</v>
+      </c>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A17:H17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>